<commit_message>
Read multiple values from one column
</commit_message>
<xml_diff>
--- a/tests/Data/Disks/Local/import-users-with-columns.xlsx
+++ b/tests/Data/Disks/Local/import-users-with-columns.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickbrouwers/Sites/Laravel-Excel/tests/Data/Disks/Local/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE3D24E9-61B7-9B4C-BD33-18712B776070}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10191808-2B33-F245-8D76-7C2AFD2A721C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="25600" yWindow="6300" windowWidth="25600" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
   <si>
     <t>patrick@maatwebsite.nl</t>
   </si>
@@ -77,14 +77,20 @@
       <t xml:space="preserve"> test</t>
     </r>
   </si>
+  <si>
+    <t>Maatwebsite</t>
+  </si>
+  <si>
+    <t>Laravel</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="166" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
+    <numFmt numFmtId="165" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -97,11 +103,13 @@
       <sz val="11"/>
       <color theme="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -142,10 +150,10 @@
   <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
@@ -453,10 +461,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="B1:L2"/>
+  <dimension ref="B1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -469,9 +477,10 @@
     <col min="6" max="6" width="14.5" style="5" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" style="3"/>
+    <col min="13" max="13" width="10.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B1" t="s">
         <v>2</v>
       </c>
@@ -504,8 +513,11 @@
       <c r="L1" s="6" t="s">
         <v>4</v>
       </c>
+      <c r="M1" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="2:13" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
         <v>3</v>
       </c>
@@ -537,6 +549,9 @@
       </c>
       <c r="L2" s="6" t="s">
         <v>5</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>
@@ -544,6 +559,8 @@
   <hyperlinks>
     <hyperlink ref="C1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
     <hyperlink ref="C2" r:id="rId2" xr:uid="{00000000-0004-0000-0000-000001000000}"/>
+    <hyperlink ref="M1" r:id="rId3" xr:uid="{71932B35-D5DD-CF40-9F7C-2D560D363CF5}"/>
+    <hyperlink ref="M2" r:id="rId4" xr:uid="{C52FAAF8-7794-904D-8422-1375D57643DC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>

<commit_message>
Add reading images from columns
</commit_message>
<xml_diff>
--- a/tests/Data/Disks/Local/import-users-with-columns.xlsx
+++ b/tests/Data/Disks/Local/import-users-with-columns.xlsx
@@ -1,90 +1,3 @@
-
-<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10411"/>
-  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickbrouwers/Sites/Laravel-Excel/tests/Data/Disks/Local/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10191808-2B33-F245-8D76-7C2AFD2A721C}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
-  <bookViews>
-    <workbookView xWindow="25600" yWindow="6300" windowWidth="25600" windowHeight="15620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
-  </bookViews>
-  <sheets>
-    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
-  </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
-</workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
-  <si>
-    <t>patrick@maatwebsite.nl</t>
-  </si>
-  <si>
-    <t>taylor@laravel.com</t>
-  </si>
-  <si>
-    <t>Patrick Brouwers</t>
-  </si>
-  <si>
-    <t>Taylor Otwell</t>
-  </si>
-  <si>
-    <t>true</t>
-  </si>
-  <si>
-    <t>false</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">test </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t>bold</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> test</t>
-    </r>
-  </si>
-  <si>
-    <t>Maatwebsite</t>
-  </si>
-  <si>
-    <t>Laravel</t>
-  </si>
-</sst>
-</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
@@ -464,7 +377,7 @@
   <dimension ref="B1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+      <selection activeCell="V7" sqref="V7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -478,6 +391,7 @@
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="8.83203125" style="3"/>
     <col min="13" max="13" width="10.83203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="28.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.2">
@@ -563,6 +477,7 @@
     <hyperlink ref="M2" r:id="rId4" xr:uid="{C52FAAF8-7794-904D-8422-1375D57643DC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId5"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>

<commit_message>
Fix xlsx test file
</commit_message>
<xml_diff>
--- a/tests/Data/Disks/Local/import-users-with-columns.xlsx
+++ b/tests/Data/Disks/Local/import-users-with-columns.xlsx
@@ -382,16 +382,17 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.6640625" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.6640625" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.1640625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="20" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.83203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="14.5" style="5" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" style="5" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.83203125" style="3"/>
+    <col min="9" max="9" width="2.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.83203125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="28.1640625" customWidth="1"/>
+    <col min="14" max="14" width="6.1640625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:13" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Fix line endings in xlsx
</commit_message>
<xml_diff>
--- a/tests/Data/Disks/Local/import-users-with-columns.xlsx
+++ b/tests/Data/Disks/Local/import-users-with-columns.xlsx
@@ -1,34 +1,228 @@
+
+<file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="10411"/>
+  <workbookPr codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/patrickbrouwers/Sites/Laravel-Excel/tests/Data/Disks/Local/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{FEAE73D7-2393-544E-A4FE-105179210C57}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <bookViews>
+    <workbookView xWindow="9460" yWindow="4460" windowWidth="41740" windowHeight="17460" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+  </bookViews>
+  <sheets>
+    <sheet name="Worksheet" sheetId="1" r:id="rId1"/>
+  </sheets>
+  <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
+</workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="9">
+  <si>
+    <t>patrick@maatwebsite.nl</t>
+  </si>
+  <si>
+    <t>taylor@laravel.com</t>
+  </si>
+  <si>
+    <t>Patrick Brouwers</t>
+  </si>
+  <si>
+    <t>Taylor Otwell</t>
+  </si>
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>false</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">test </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>bold</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> test</t>
+    </r>
+  </si>
+  <si>
+    <t>Maatwebsite</t>
+  </si>
+  <si>
+    <t>Laravel</t>
+  </si>
+</sst>
+</file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="[$-F800]dddd\,\ mmmm\ dd\,\ yyyy"/>
-    <numFmt numFmtId="165" formatCode="_([$€-2]\ * #,##0.00_);_([$€-2]\ * \(#,##0.00\);_([$€-2]\ * &quot;-&quot;??_);_(@_)"/>
-  </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
-    <font>
+  <fonts count="20" x14ac:knownFonts="1">
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Cambria"/>
+      <family val="2"/>
+      <scheme val="major"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="12"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -37,16 +231,195 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="65"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -54,28 +427,207 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Procent" xfId="2" builtinId="5"/>
+  <cellStyles count="42">
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
+    <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
+    <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
+    <cellStyle name="20% - Accent4" xfId="31" builtinId="42" customBuiltin="1"/>
+    <cellStyle name="20% - Accent5" xfId="35" builtinId="46" customBuiltin="1"/>
+    <cellStyle name="20% - Accent6" xfId="39" builtinId="50" customBuiltin="1"/>
+    <cellStyle name="40% - Accent1" xfId="20" builtinId="31" customBuiltin="1"/>
+    <cellStyle name="40% - Accent2" xfId="24" builtinId="35" customBuiltin="1"/>
+    <cellStyle name="40% - Accent3" xfId="28" builtinId="39" customBuiltin="1"/>
+    <cellStyle name="40% - Accent4" xfId="32" builtinId="43" customBuiltin="1"/>
+    <cellStyle name="40% - Accent5" xfId="36" builtinId="47" customBuiltin="1"/>
+    <cellStyle name="40% - Accent6" xfId="40" builtinId="51" customBuiltin="1"/>
+    <cellStyle name="60% - Accent1" xfId="21" builtinId="32" customBuiltin="1"/>
+    <cellStyle name="60% - Accent2" xfId="25" builtinId="36" customBuiltin="1"/>
+    <cellStyle name="60% - Accent3" xfId="29" builtinId="40" customBuiltin="1"/>
+    <cellStyle name="60% - Accent4" xfId="33" builtinId="44" customBuiltin="1"/>
+    <cellStyle name="60% - Accent5" xfId="37" builtinId="48" customBuiltin="1"/>
+    <cellStyle name="60% - Accent6" xfId="41" builtinId="52" customBuiltin="1"/>
+    <cellStyle name="Accent1" xfId="18" builtinId="29" customBuiltin="1"/>
+    <cellStyle name="Accent2" xfId="22" builtinId="33" customBuiltin="1"/>
+    <cellStyle name="Accent3" xfId="26" builtinId="37" customBuiltin="1"/>
+    <cellStyle name="Accent4" xfId="30" builtinId="41" customBuiltin="1"/>
+    <cellStyle name="Accent5" xfId="34" builtinId="45" customBuiltin="1"/>
+    <cellStyle name="Accent6" xfId="38" builtinId="49" customBuiltin="1"/>
+    <cellStyle name="Berekening" xfId="11" builtinId="22" customBuiltin="1"/>
+    <cellStyle name="Controlecel" xfId="13" builtinId="23" customBuiltin="1"/>
+    <cellStyle name="Gekoppelde cel" xfId="12" builtinId="24" customBuiltin="1"/>
+    <cellStyle name="Goed" xfId="6" builtinId="26" customBuiltin="1"/>
+    <cellStyle name="Invoer" xfId="9" builtinId="20" customBuiltin="1"/>
+    <cellStyle name="Kop 1" xfId="2" builtinId="16" customBuiltin="1"/>
+    <cellStyle name="Kop 2" xfId="3" builtinId="17" customBuiltin="1"/>
+    <cellStyle name="Kop 3" xfId="4" builtinId="18" customBuiltin="1"/>
+    <cellStyle name="Kop 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Neutraal" xfId="8" builtinId="28" customBuiltin="1"/>
+    <cellStyle name="Notitie" xfId="15" builtinId="10" customBuiltin="1"/>
+    <cellStyle name="Ongeldig" xfId="7" builtinId="27" customBuiltin="1"/>
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
+    <cellStyle name="Titel" xfId="1" builtinId="15" customBuiltin="1"/>
+    <cellStyle name="Totaal" xfId="17" builtinId="25" customBuiltin="1"/>
+    <cellStyle name="Uitvoer" xfId="10" builtinId="21" customBuiltin="1"/>
+    <cellStyle name="Verklarende tekst" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Waarschuwingstekst" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -85,6 +637,99 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>17780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="6" name="Afbeelding 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{601E82C2-0F26-FA48-ADE1-BE9DC1AE8883}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11023600" y="203200"/>
+          <a:ext cx="368300" cy="220980"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>368300</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>17780</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="8" name="Afbeelding 7">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C40E34A2-644A-FA43-8D21-AC7B10400F4E}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11023600" y="0"/>
+          <a:ext cx="368300" cy="220980"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -377,19 +1022,19 @@
   <dimension ref="B1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="V7" sqref="V7"/>
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="5.6640625" customWidth="1"/>
     <col min="2" max="2" width="19.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.6640625" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.83203125" style="4" customWidth="1"/>
-    <col min="6" max="6" width="5.33203125" style="5" customWidth="1"/>
+    <col min="3" max="3" width="20" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.83203125" customWidth="1"/>
+    <col min="6" max="6" width="5.33203125" customWidth="1"/>
     <col min="8" max="8" width="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="2.1640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="2.1640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="11" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="10.83203125" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="6.1640625" customWidth="1"/>
@@ -399,36 +1044,35 @@
       <c r="B1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="2">
+      <c r="D1">
         <v>34007</v>
       </c>
-      <c r="E1" s="3">
+      <c r="E1">
         <v>1000</v>
       </c>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4">
+      <c r="G1">
         <v>1</v>
       </c>
-      <c r="H1" s="5">
+      <c r="H1">
         <v>100</v>
       </c>
       <c r="I1">
         <f>1+1</f>
         <v>2</v>
       </c>
-      <c r="J1" s="6" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="3">
+      <c r="K1">
         <v>10.5</v>
       </c>
-      <c r="L1" s="6" t="s">
+      <c r="L1" t="s">
         <v>4</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="M1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -436,36 +1080,35 @@
       <c r="B2" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="2">
+      <c r="D2">
         <v>31560</v>
       </c>
-      <c r="E2" s="3">
+      <c r="E2">
         <v>2000</v>
       </c>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4">
+      <c r="G2">
         <v>2</v>
       </c>
-      <c r="H2" s="5">
+      <c r="H2">
         <v>200</v>
       </c>
       <c r="I2">
         <f>2+3</f>
         <v>5</v>
       </c>
-      <c r="J2" s="6" t="s">
+      <c r="J2" t="s">
         <v>6</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2">
         <v>20.5</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" t="s">
         <v>5</v>
       </c>
-      <c r="M2" s="1" t="s">
+      <c r="M2" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>